<commit_message>
bug fix on MDZ logos try except for new registered persons
</commit_message>
<xml_diff>
--- a/mdz_Logo_Pfad.xlsx
+++ b/mdz_Logo_Pfad.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\km\Desktop\Namensschild_app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\km\Desktop\label-printer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E791B4-E699-4DB1-9A8A-6D952277F060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3418AF-5060-486F-A72D-FBB59DF69D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50745" yWindow="-4425" windowWidth="14295" windowHeight="15225" xr2:uid="{698B21B6-113F-4ABD-BFA9-CDDE870831E8}"/>
+    <workbookView minimized="1" xWindow="3640" yWindow="790" windowWidth="14400" windowHeight="7270" xr2:uid="{698B21B6-113F-4ABD-BFA9-CDDE870831E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle3" sheetId="3" r:id="rId1"/>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C603CD-A63E-4622-820C-98DE86A7D0F8}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>